<commit_message>
refactor, fix minor issues
</commit_message>
<xml_diff>
--- a/api/src/assets/drydock/Yard Quotation Template.xlsx
+++ b/api/src/assets/drydock/Yard Quotation Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basujitchakravarty/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CA77CA2-1974-4F95-8927-20F9AAEE1B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9608893-D0AE-4E28-A7F1-9C53D27DADD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22360" xr2:uid="{384ECE5B-D30A-8C45-BF66-8C857F5405C5}"/>
   </bookViews>
@@ -40,143 +40,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={8FB7F143-D7F9-463D-A29F-B13B723F1063}</author>
-    <author>tc={BE81286B-C943-46F9-B50F-CA7A9DDE5B19}</author>
-    <author>tc={E29AA953-CC19-42E7-8752-5AA0284EA37B}</author>
-    <author>tc={B5DC3CCD-154A-4DCC-B5BC-8DB279922C87}</author>
-    <author>tc={FAAEC501-0C64-4D0A-A6F6-DB3EF2CB1435}</author>
-    <author>tc={D663BC33-B7E8-4837-AAAD-6369050C454D}</author>
-    <author>tc={1C1C737D-AF71-48FD-A319-A7BB5872EDD8}</author>
-    <author>tc={9CD55D98-328E-4E1E-88A7-CC9E82A4674C}</author>
-    <author>tc={4AB38907-F846-490D-8BDD-5BD7B6BED039}</author>
-    <author>tc={4BE4FBAE-3645-4588-AD10-1F355EF0919D}</author>
-    <author>tc={E86D379B-22AC-44A7-B676-6483581EA71A}</author>
-    <author>tc={C1EB3BE9-DA73-48E7-B074-7F9A7FDA3AB6}</author>
-    <author>tc={8DC96B5A-40B6-4EF1-B654-3A49B3D05DDF}</author>
-    <author>tc={C040FCDD-0774-46C5-B577-389090719AE6}</author>
-  </authors>
-  <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{8FB7F143-D7F9-463D-A29F-B13B723F1063}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    General Notes and conditions that can be different per client</t>
-      </text>
-    </comment>
-    <comment ref="C8" authorId="1" shapeId="0" xr:uid="{BE81286B-C943-46F9-B50F-CA7A9DDE5B19}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Management Company of the Vessel from the Vessel Library</t>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="2" shapeId="0" xr:uid="{E29AA953-CC19-42E7-8752-5AA0284EA37B}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Yard will enter any remarks regarding the quotation here. Free text</t>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="3" shapeId="0" xr:uid="{B5DC3CCD-154A-4DCC-B5BC-8DB279922C87}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Shipyard selected within JiBe dry docking</t>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="4" shapeId="0" xr:uid="{FAAEC501-0C64-4D0A-A6F6-DB3EF2CB1435}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Subject of the dry docking project</t>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="5" shapeId="0" xr:uid="{D663BC33-B7E8-4837-AAAD-6369050C454D}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Date From and Date To for the Dry docking project at the time of export</t>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="6" shapeId="0" xr:uid="{1C1C737D-AF71-48FD-A319-A7BB5872EDD8}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    List of selectable currencies from the allowed currency list / Company Registry yard contact card allowed currency list</t>
-      </text>
-    </comment>
-    <comment ref="H12" authorId="7" shapeId="0" xr:uid="{9CD55D98-328E-4E1E-88A7-CC9E82A4674C}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Total cost calculated from the sum of all Job Totals</t>
-      </text>
-    </comment>
-    <comment ref="I12" authorId="8" shapeId="0" xr:uid="{4AB38907-F846-490D-8BDD-5BD7B6BED039}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Currency selected by the yard for the quotation</t>
-      </text>
-    </comment>
-    <comment ref="C13" authorId="9" shapeId="0" xr:uid="{4BE4FBAE-3645-4588-AD10-1F355EF0919D}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Overall Discount / Applied after calculating the total of all specifications</t>
-      </text>
-    </comment>
-    <comment ref="H13" authorId="10" shapeId="0" xr:uid="{E86D379B-22AC-44A7-B676-6483581EA71A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Overall discount calculated value when applied to the Gross Total</t>
-      </text>
-    </comment>
-    <comment ref="C14" authorId="11" shapeId="0" xr:uid="{C1EB3BE9-DA73-48E7-B074-7F9A7FDA3AB6}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    A dry docking project usually involves days at anchor / berth which does not incur wharfage but contribute to the overall duration of the vessel stay in the yard. Expects an input in number of days</t>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="12" shapeId="0" xr:uid="{8DC96B5A-40B6-4EF1-B654-3A49B3D05DDF}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Calculated Total = Gross Total - Overall Discount</t>
-      </text>
-    </comment>
-    <comment ref="C15" authorId="13" shapeId="0" xr:uid="{C040FCDD-0774-46C5-B577-389090719AE6}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Dock Days is the expected stay in the dry docking during the yard stay. Expects an input in number of days</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>SHIPYARD QUOTATION TEMPLATE</t>
   </si>
@@ -200,9 +65,6 @@
   </si>
   <si>
     <t>MANAGEMENT COMPANY</t>
-  </si>
-  <si>
-    <t>Quotation is provided basis our standard terms and conditions found here - www.keppel.com/terms.</t>
   </si>
   <si>
     <t>YARD</t>
@@ -282,7 +144,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.00\ _k_r_.;[Red]#,##0.00\ _k_r_."/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ _k_r_.;[Red]#,##0.00\ _k_r_."/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -687,7 +549,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -697,7 +559,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -705,15 +567,6 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -765,6 +618,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -840,12 +702,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Basujit Chakravarty (Product/DK)" id="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" userId="S::basujit.chakravarty@jibe.solutions::4ad117ac-26e0-4069-9c5f-a4d88bf45a9e" providerId="AD"/>
-</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1163,63 +1019,16 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C3" dT="2023-11-06T18:08:41.97" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{8FB7F143-D7F9-463D-A29F-B13B723F1063}">
-    <text>General Notes and conditions that can be different per client</text>
-  </threadedComment>
-  <threadedComment ref="C8" dT="2023-11-06T18:10:21.60" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{BE81286B-C943-46F9-B50F-CA7A9DDE5B19}">
-    <text>Management Company of the Vessel from the Vessel Library</text>
-  </threadedComment>
-  <threadedComment ref="D8" dT="2023-11-06T18:25:40.50" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{E29AA953-CC19-42E7-8752-5AA0284EA37B}">
-    <text>Yard will enter any remarks regarding the quotation here. Free text</text>
-  </threadedComment>
-  <threadedComment ref="C9" dT="2023-11-06T18:11:07.27" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{B5DC3CCD-154A-4DCC-B5BC-8DB279922C87}">
-    <text>Shipyard selected within JiBe dry docking</text>
-  </threadedComment>
-  <threadedComment ref="C10" dT="2023-11-06T18:11:17.58" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{FAAEC501-0C64-4D0A-A6F6-DB3EF2CB1435}">
-    <text>Subject of the dry docking project</text>
-  </threadedComment>
-  <threadedComment ref="C11" dT="2023-11-06T18:11:32.10" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{D663BC33-B7E8-4837-AAAD-6369050C454D}">
-    <text>Date From and Date To for the Dry docking project at the time of export</text>
-  </threadedComment>
-  <threadedComment ref="C12" dT="2023-11-06T18:13:27.48" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{1C1C737D-AF71-48FD-A319-A7BB5872EDD8}">
-    <text>List of selectable currencies from the allowed currency list / Company Registry yard contact card allowed currency list</text>
-  </threadedComment>
-  <threadedComment ref="H12" dT="2023-11-06T18:26:00.44" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{9CD55D98-328E-4E1E-88A7-CC9E82A4674C}">
-    <text>Total cost calculated from the sum of all Job Totals</text>
-  </threadedComment>
-  <threadedComment ref="I12" dT="2023-11-06T18:27:39.43" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{4AB38907-F846-490D-8BDD-5BD7B6BED039}">
-    <text>Currency selected by the yard for the quotation</text>
-  </threadedComment>
-  <threadedComment ref="C13" dT="2023-11-06T18:13:53.96" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{4BE4FBAE-3645-4588-AD10-1F355EF0919D}">
-    <text>Overall Discount / Applied after calculating the total of all specifications</text>
-  </threadedComment>
-  <threadedComment ref="H13" dT="2023-11-06T18:26:23.42" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{E86D379B-22AC-44A7-B676-6483581EA71A}">
-    <text>Overall discount calculated value when applied to the Gross Total</text>
-  </threadedComment>
-  <threadedComment ref="C14" dT="2023-11-06T18:14:40.40" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{C1EB3BE9-DA73-48E7-B074-7F9A7FDA3AB6}">
-    <text>A dry docking project usually involves days at anchor / berth which does not incur wharfage but contribute to the overall duration of the vessel stay in the yard. Expects an input in number of days</text>
-  </threadedComment>
-  <threadedComment ref="H14" dT="2023-11-06T18:27:27.78" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{8DC96B5A-40B6-4EF1-B654-3A49B3D05DDF}">
-    <text>Calculated Total = Gross Total - Overall Discount</text>
-  </threadedComment>
-  <threadedComment ref="C15" dT="2023-11-06T18:15:14.24" personId="{D5F1E22A-5E86-438E-9EC4-D565D29E2BE8}" id="{C040FCDD-0774-46C5-B577-389090719AE6}">
-    <text>Dock Days is the expected stay in the dry docking during the yard stay. Expects an input in number of days</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63955BAE-A3D8-D744-8971-FF2F527A39DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63955BAE-A3D8-D744-8971-FF2F527A39DB}">
   <sheetPr codeName="Sheet8">
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="B1:J98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="135" workbookViewId="0">
-      <pane xSplit="1" ySplit="16" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <pane xSplit="1" ySplit="16" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -1241,61 +1050,61 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14.1" thickBot="1"/>
     <row r="2" spans="2:10" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="35"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B3" s="45"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="40"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="37"/>
       <c r="J3" s="13"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B4" s="46"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B5" s="46"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="42"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="13"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B6" s="47"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="13"/>
     </row>
     <row r="7" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1305,14 +1114,14 @@
       <c r="C7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
       <c r="J7" s="16"/>
     </row>
     <row r="8" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1322,52 +1131,50 @@
       <c r="C8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="38"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
       <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="38"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="35"/>
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
       <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="35"/>
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
       <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>13</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="22"/>
@@ -1379,17 +1186,17 @@
     </row>
     <row r="12" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
       <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="48"/>
+      <c r="F12" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="45"/>
       <c r="H12" s="24">
         <v>0</v>
       </c>
@@ -1401,17 +1208,17 @@
     </row>
     <row r="13" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="26">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="48"/>
+      <c r="F13" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="45"/>
       <c r="H13" s="27">
         <f>C13*H12*(-1)</f>
         <v>0</v>
@@ -1424,17 +1231,15 @@
     </row>
     <row r="14" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
       <c r="B14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="10">
-        <v>7</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C14" s="10"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="48"/>
+      <c r="F14" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="45"/>
       <c r="H14" s="24">
         <f>H12+H13</f>
         <v>0</v>
@@ -1447,11 +1252,9 @@
     </row>
     <row r="15" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1" thickBot="1">
       <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="11">
-        <v>5</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C15" s="11"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1462,28 +1265,28 @@
     </row>
     <row r="16" spans="2:10" s="18" customFormat="1" ht="27.95" customHeight="1">
       <c r="B16" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="D16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="E16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="F16" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="G16" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="H16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="I16" s="20" t="s">
         <v>28</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:9" s="18" customFormat="1" ht="30" customHeight="1">
@@ -1579,19 +1382,18 @@
     <row r="98" ht="12.75"/>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D7:I7"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="D8:I10"/>
     <mergeCell ref="C3:I6"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
@@ -1619,17 +1421,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1639,26 +1441,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="213ede84-1d54-4469-9df9-7f5044be5c73">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b5f0b2fe-13ea-4965-a1f0-cfe54b2bf3fc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045EB93BC68A14742BC74ADCE8022DFED" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9bae4091dc7f3d3aa07b0af249c4c9c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="213ede84-1d54-4469-9df9-7f5044be5c73" xmlns:ns3="b5f0b2fe-13ea-4965-a1f0-cfe54b2bf3fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19db3f51d7fc962c8baae4fdf64f124d" ns2:_="" ns3:_="">
     <xsd:import namespace="213ede84-1d54-4469-9df9-7f5044be5c73"/>
@@ -1881,8 +1663,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="213ede84-1d54-4469-9df9-7f5044be5c73">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b5f0b2fe-13ea-4965-a1f0-cfe54b2bf3fc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{790806D0-957C-4E2C-95E1-601B20718C24}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95611AF2-4575-4FD9-A624-4C87522C6067}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1890,5 +1692,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95611AF2-4575-4FD9-A624-4C87522C6067}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{790806D0-957C-4E2C-95E1-601B20718C24}"/>
 </file>
</xml_diff>

<commit_message>
fixed currency flow as we discussed
</commit_message>
<xml_diff>
--- a/api/src/assets/drydock/Yard Quotation Template.xlsx
+++ b/api/src/assets/drydock/Yard Quotation Template.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basujitchakravarty/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9608893-D0AE-4E28-A7F1-9C53D27DADD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF2B83DA-B19C-49AE-B32F-EA082E92A204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22360" xr2:uid="{384ECE5B-D30A-8C45-BF66-8C857F5405C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Quotation Template" sheetId="1" r:id="rId1"/>
-    <sheet name="Libraries" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Currency">'Quotation Template'!$C$12:$C$12</definedName>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>SHIPYARD QUOTATION TEMPLATE</t>
   </si>
@@ -88,9 +87,6 @@
     <t>CURRENCY</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>GROSS TOTAL</t>
   </si>
   <si>
@@ -131,12 +127,6 @@
   </si>
   <si>
     <t>YARD COMMENTS</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>SGD</t>
   </si>
 </sst>
 </file>
@@ -568,6 +558,18 @@
     <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -615,18 +617,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1027,8 +1017,8 @@
   <dimension ref="B1:J98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="135" workbookViewId="0">
-      <pane xSplit="1" ySplit="16" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <pane xSplit="1" ySplit="16" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -1050,61 +1040,61 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14.1" thickBot="1"/>
     <row r="2" spans="2:10" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B3" s="42"/>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="37"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="13"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B4" s="43"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B5" s="43"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="39"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="43"/>
       <c r="J5" s="13"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B6" s="44"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="13"/>
     </row>
     <row r="7" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1114,14 +1104,14 @@
       <c r="C7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="48"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
       <c r="J7" s="16"/>
     </row>
     <row r="8" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1131,12 +1121,12 @@
       <c r="C8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1146,12 +1136,12 @@
       <c r="C9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="39"/>
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1161,12 +1151,12 @@
       <c r="C10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1188,71 +1178,69 @@
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="C12" s="10"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="45"/>
+      <c r="F12" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="30"/>
       <c r="H12" s="24">
         <v>0</v>
       </c>
       <c r="I12" s="6" t="str">
         <f>IF(ISBLANK(C12),"",C12)</f>
-        <v>EUR</v>
+        <v/>
       </c>
       <c r="J12" s="16"/>
     </row>
     <row r="13" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="26">
         <v>0</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="45"/>
+      <c r="F13" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="30"/>
       <c r="H13" s="27">
         <f>C13*H12*(-1)</f>
         <v>0</v>
       </c>
       <c r="I13" s="6" t="str">
         <f>IF(ISBLANK(C12),"",C12)</f>
-        <v>EUR</v>
+        <v/>
       </c>
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="45"/>
+      <c r="F14" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="30"/>
       <c r="H14" s="24">
         <f>H12+H13</f>
         <v>0</v>
       </c>
       <c r="I14" s="6" t="str">
         <f>IF(ISBLANK(C12),"",C12)</f>
-        <v>EUR</v>
+        <v/>
       </c>
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1" thickBot="1">
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="7"/>
@@ -1265,28 +1253,28 @@
     </row>
     <row r="16" spans="2:10" s="18" customFormat="1" ht="27.95" customHeight="1">
       <c r="B16" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="D16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="E16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="F16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="G16" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="H16" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="I16" s="20" t="s">
         <v>27</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:9" s="18" customFormat="1" ht="30" customHeight="1">
@@ -1391,56 +1379,27 @@
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="F12:G12"/>
   </mergeCells>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{1606D3EB-7C92-504C-84E7-C9D8C8168B90}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1606D3EB-7C92-504C-84E7-C9D8C8168B90}">
-          <x14:formula1>
-            <xm:f>Libraries!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>C12</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15560984-1AE8-D741-88A8-3A1FBA6E209C}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView zoomScale="194" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.95"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="213ede84-1d54-4469-9df9-7f5044be5c73">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b5f0b2fe-13ea-4965-a1f0-cfe54b2bf3fc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045EB93BC68A14742BC74ADCE8022DFED" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9bae4091dc7f3d3aa07b0af249c4c9c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="213ede84-1d54-4469-9df9-7f5044be5c73" xmlns:ns3="b5f0b2fe-13ea-4965-a1f0-cfe54b2bf3fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19db3f51d7fc962c8baae4fdf64f124d" ns2:_="" ns3:_="">
     <xsd:import namespace="213ede84-1d54-4469-9df9-7f5044be5c73"/>
@@ -1663,7 +1622,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1672,25 +1631,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="213ede84-1d54-4469-9df9-7f5044be5c73">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b5f0b2fe-13ea-4965-a1f0-cfe54b2bf3fc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{790806D0-957C-4E2C-95E1-601B20718C24}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95611AF2-4575-4FD9-A624-4C87522C6067}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70C681E6-9A1D-4313-8207-23814A13B26D}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{790806D0-957C-4E2C-95E1-601B20718C24}"/>
 </file>
</xml_diff>

<commit_message>
Merged PR 87865: fixed currency flow as we discussed
Related work items: #662930
</commit_message>
<xml_diff>
--- a/api/src/assets/drydock/Yard Quotation Template.xlsx
+++ b/api/src/assets/drydock/Yard Quotation Template.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basujitchakravarty/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9608893-D0AE-4E28-A7F1-9C53D27DADD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF2B83DA-B19C-49AE-B32F-EA082E92A204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22360" xr2:uid="{384ECE5B-D30A-8C45-BF66-8C857F5405C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Quotation Template" sheetId="1" r:id="rId1"/>
-    <sheet name="Libraries" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Currency">'Quotation Template'!$C$12:$C$12</definedName>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>SHIPYARD QUOTATION TEMPLATE</t>
   </si>
@@ -88,9 +87,6 @@
     <t>CURRENCY</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>GROSS TOTAL</t>
   </si>
   <si>
@@ -131,12 +127,6 @@
   </si>
   <si>
     <t>YARD COMMENTS</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>SGD</t>
   </si>
 </sst>
 </file>
@@ -568,6 +558,18 @@
     <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -615,18 +617,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1027,8 +1017,8 @@
   <dimension ref="B1:J98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="135" workbookViewId="0">
-      <pane xSplit="1" ySplit="16" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <pane xSplit="1" ySplit="16" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -1050,61 +1040,61 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14.1" thickBot="1"/>
     <row r="2" spans="2:10" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B3" s="42"/>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="37"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="13"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B4" s="43"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B5" s="43"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="39"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="43"/>
       <c r="J5" s="13"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B6" s="44"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="13"/>
     </row>
     <row r="7" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1114,14 +1104,14 @@
       <c r="C7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="48"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
       <c r="J7" s="16"/>
     </row>
     <row r="8" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1131,12 +1121,12 @@
       <c r="C8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1146,12 +1136,12 @@
       <c r="C9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="39"/>
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1161,12 +1151,12 @@
       <c r="C10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
@@ -1188,71 +1178,69 @@
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="C12" s="10"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="45"/>
+      <c r="F12" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="30"/>
       <c r="H12" s="24">
         <v>0</v>
       </c>
       <c r="I12" s="6" t="str">
         <f>IF(ISBLANK(C12),"",C12)</f>
-        <v>EUR</v>
+        <v/>
       </c>
       <c r="J12" s="16"/>
     </row>
     <row r="13" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="26">
         <v>0</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="45"/>
+      <c r="F13" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="30"/>
       <c r="H13" s="27">
         <f>C13*H12*(-1)</f>
         <v>0</v>
       </c>
       <c r="I13" s="6" t="str">
         <f>IF(ISBLANK(C12),"",C12)</f>
-        <v>EUR</v>
+        <v/>
       </c>
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="45"/>
+      <c r="F14" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="30"/>
       <c r="H14" s="24">
         <f>H12+H13</f>
         <v>0</v>
       </c>
       <c r="I14" s="6" t="str">
         <f>IF(ISBLANK(C12),"",C12)</f>
-        <v>EUR</v>
+        <v/>
       </c>
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1" thickBot="1">
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="7"/>
@@ -1265,28 +1253,28 @@
     </row>
     <row r="16" spans="2:10" s="18" customFormat="1" ht="27.95" customHeight="1">
       <c r="B16" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="D16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="E16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="F16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="G16" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="H16" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="I16" s="20" t="s">
         <v>27</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:9" s="18" customFormat="1" ht="30" customHeight="1">
@@ -1391,56 +1379,27 @@
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="F12:G12"/>
   </mergeCells>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{1606D3EB-7C92-504C-84E7-C9D8C8168B90}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1606D3EB-7C92-504C-84E7-C9D8C8168B90}">
-          <x14:formula1>
-            <xm:f>Libraries!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>C12</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15560984-1AE8-D741-88A8-3A1FBA6E209C}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView zoomScale="194" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.95"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="213ede84-1d54-4469-9df9-7f5044be5c73">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b5f0b2fe-13ea-4965-a1f0-cfe54b2bf3fc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045EB93BC68A14742BC74ADCE8022DFED" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9bae4091dc7f3d3aa07b0af249c4c9c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="213ede84-1d54-4469-9df9-7f5044be5c73" xmlns:ns3="b5f0b2fe-13ea-4965-a1f0-cfe54b2bf3fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19db3f51d7fc962c8baae4fdf64f124d" ns2:_="" ns3:_="">
     <xsd:import namespace="213ede84-1d54-4469-9df9-7f5044be5c73"/>
@@ -1663,7 +1622,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1672,25 +1631,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="213ede84-1d54-4469-9df9-7f5044be5c73">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b5f0b2fe-13ea-4965-a1f0-cfe54b2bf3fc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{790806D0-957C-4E2C-95E1-601B20718C24}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95611AF2-4575-4FD9-A624-4C87522C6067}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70C681E6-9A1D-4313-8207-23814A13B26D}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{790806D0-957C-4E2C-95E1-601B20718C24}"/>
 </file>
</xml_diff>

<commit_message>
Merged PR 88501: fix template
Related work items: #662930
</commit_message>
<xml_diff>
--- a/api/src/assets/drydock/Yard Quotation Template.xlsx
+++ b/api/src/assets/drydock/Yard Quotation Template.xlsx
@@ -1,24 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27226"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basujitchakravarty/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF2B83DA-B19C-49AE-B32F-EA082E92A204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27230"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCBC96E8-E038-443D-8F88-84780BC16CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22360" xr2:uid="{384ECE5B-D30A-8C45-BF66-8C857F5405C5}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quotation Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="Currency">'Quotation Template'!$C$12:$C$12</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Quotation Template'!$A:$J</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -136,17 +127,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ _k_r_.;[Red]#,##0.00\ _k_r_."/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -166,7 +151,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Nirmala UI"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -217,13 +202,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.89999084444715716"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -235,13 +214,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3"/>
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -252,6 +237,189 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -280,360 +448,164 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="4" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{0798CF28-5EB0-044D-AC5E-B0EA524B5EAD}"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="3" xr:uid="{E69EE76F-ED78-D944-8A94-488639A21A95}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFBEF94E"/>
-      <color rgb="FFDCE9F9"/>
-      <color rgb="FFDBE9F9"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -650,22 +622,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>119944</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1549400</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1584325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>194381</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CA708B4-C33C-191D-AD3B-2822ED1E7FB9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -674,15 +646,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="826441" y="486833"/>
-          <a:ext cx="1155700" cy="444500"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -705,39 +677,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -789,7 +761,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -900,6 +872,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -908,13 +887,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -979,412 +951,315 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63955BAE-A3D8-D744-8971-FF2F527A39DB}">
-  <sheetPr codeName="Sheet8">
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="B1:J98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="135" workbookViewId="0">
-      <pane xSplit="1" ySplit="16" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="58.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="12" style="12" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" style="12" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="58.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="14.1" thickBot="1"/>
-    <row r="2" spans="2:10" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="B2" s="34" t="s">
+    <row r="1" spans="1:10" ht="14.1" customHeight="1"/>
+    <row r="2" spans="1:10" ht="30" customHeight="1">
+      <c r="A2" s="1"/>
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B3" s="46"/>
-      <c r="C3" s="40" t="s">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="13"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B4" s="47"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="13"/>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B5" s="47"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="13"/>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B6" s="48"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="13"/>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:10" ht="12.95" customHeight="1">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="16"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:10" ht="12.95" customHeight="1">
+      <c r="A8" s="4"/>
+      <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="16"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:10" ht="12.95" customHeight="1">
+      <c r="A9" s="4"/>
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="16"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:10" ht="12.95" customHeight="1">
+      <c r="A10" s="4"/>
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="16"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="1:10" ht="12.95" customHeight="1">
+      <c r="A11" s="4"/>
+      <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="16"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="1:10" ht="12.95" customHeight="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="30" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="30"/>
-      <c r="H12" s="24">
+      <c r="H12" s="21">
         <v>0</v>
       </c>
-      <c r="I12" s="6" t="str">
+      <c r="I12" s="22" t="str">
         <f>IF(ISBLANK(C12),"",C12)</f>
         <v/>
       </c>
-      <c r="J12" s="16"/>
+      <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="1:10" ht="12.95" customHeight="1">
+      <c r="A13" s="4"/>
+      <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="28">
         <v>0</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="30"/>
-      <c r="H13" s="27">
+      <c r="H13" s="23">
         <f>C13*H12*(-1)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="6" t="str">
+      <c r="I13" s="22" t="str">
         <f>IF(ISBLANK(C12),"",C12)</f>
         <v/>
       </c>
-      <c r="J13" s="16"/>
+      <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="1:10" ht="12.95" customHeight="1">
+      <c r="A14" s="4"/>
+      <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="30" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="30"/>
-      <c r="H14" s="24">
+      <c r="H14" s="21">
         <f>H12+H13</f>
         <v>0</v>
       </c>
-      <c r="I14" s="6" t="str">
+      <c r="I14" s="22" t="str">
         <f>IF(ISBLANK(C12),"",C12)</f>
         <v/>
       </c>
-      <c r="J14" s="16"/>
+      <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:10" s="14" customFormat="1" ht="12.95" customHeight="1" thickBot="1">
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="1:10" ht="12.95" customHeight="1">
+      <c r="A15" s="4"/>
+      <c r="B15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="16"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:10" s="18" customFormat="1" ht="27.95" customHeight="1">
-      <c r="B16" s="25" t="s">
+    <row r="16" spans="1:10" ht="27.95" customHeight="1">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:9" s="18" customFormat="1" ht="30" customHeight="1">
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
+    <row r="17" spans="1:9">
+      <c r="A17" s="11"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
     </row>
-    <row r="18" spans="2:9" ht="12.75"/>
-    <row r="19" spans="2:9" ht="12.75"/>
-    <row r="20" spans="2:9" ht="12.75"/>
-    <row r="21" spans="2:9" ht="12.75"/>
-    <row r="22" spans="2:9" ht="12.75"/>
-    <row r="23" spans="2:9" ht="12.75"/>
-    <row r="24" spans="2:9" ht="12.75"/>
-    <row r="25" spans="2:9" ht="12.75"/>
-    <row r="26" spans="2:9" ht="12.75"/>
-    <row r="27" spans="2:9" ht="12.75"/>
-    <row r="28" spans="2:9" ht="12.75"/>
-    <row r="29" spans="2:9" ht="12.75"/>
-    <row r="30" spans="2:9" ht="12.75"/>
-    <row r="31" spans="2:9" ht="12.75"/>
-    <row r="32" spans="2:9" ht="12.75"/>
-    <row r="33" ht="12.75"/>
-    <row r="34" ht="12.75"/>
-    <row r="35" ht="12.75"/>
-    <row r="36" ht="12.75"/>
-    <row r="37" ht="12.75"/>
-    <row r="38" ht="12.75"/>
-    <row r="39" ht="12.75"/>
-    <row r="40" ht="12.75"/>
-    <row r="41" ht="12.75"/>
-    <row r="42" ht="12.75"/>
-    <row r="43" ht="12.75"/>
-    <row r="44" ht="12.75"/>
-    <row r="45" ht="12.75"/>
-    <row r="46" ht="12.75"/>
-    <row r="47" ht="12.75"/>
-    <row r="48" ht="12.75"/>
-    <row r="49" ht="12.75"/>
-    <row r="50" ht="12.75"/>
-    <row r="51" ht="12.75"/>
-    <row r="52" ht="12.75"/>
-    <row r="53" ht="12.75"/>
-    <row r="54" ht="12.75"/>
-    <row r="55" ht="12.75"/>
-    <row r="56" ht="12.75"/>
-    <row r="57" ht="12.75"/>
-    <row r="58" ht="12.75"/>
-    <row r="59" ht="12.75"/>
-    <row r="60" ht="12.75"/>
-    <row r="61" ht="12.75"/>
-    <row r="62" ht="12.75"/>
-    <row r="63" ht="12.75"/>
-    <row r="64" ht="12.75"/>
-    <row r="65" ht="12.75"/>
-    <row r="66" ht="12.75"/>
-    <row r="67" ht="12.75"/>
-    <row r="68" ht="12.75"/>
-    <row r="69" ht="12.75"/>
-    <row r="70" ht="12.75"/>
-    <row r="71" ht="12.75"/>
-    <row r="72" ht="12.75"/>
-    <row r="73" ht="12.75"/>
-    <row r="74" ht="12.75"/>
-    <row r="75" ht="12.75"/>
-    <row r="76" ht="12.75"/>
-    <row r="77" ht="12.75"/>
-    <row r="78" ht="12.75"/>
-    <row r="79" ht="12.75"/>
-    <row r="80" ht="12.75"/>
-    <row r="81" ht="12.75"/>
-    <row r="82" ht="12.75"/>
-    <row r="83" ht="12.75"/>
-    <row r="84" ht="12.75"/>
-    <row r="85" ht="12.75"/>
-    <row r="86" ht="12.75"/>
-    <row r="87" ht="12.75"/>
-    <row r="88" ht="12.75"/>
-    <row r="89" ht="12.75"/>
-    <row r="90" ht="12.75"/>
-    <row r="91" ht="12.75"/>
-    <row r="92" ht="12.75"/>
-    <row r="93" ht="12.75"/>
-    <row r="94" ht="12.75"/>
-    <row r="95" ht="12.75"/>
-    <row r="96" ht="12.75"/>
-    <row r="97" ht="12.75"/>
-    <row r="98" ht="12.75"/>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
+    <mergeCell ref="C3:I6"/>
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:B6"/>
     <mergeCell ref="D8:I10"/>
-    <mergeCell ref="C3:I6"/>
-    <mergeCell ref="B3:B6"/>
     <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{1606D3EB-7C92-504C-84E7-C9D8C8168B90}"/>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1632,13 +1507,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{790806D0-957C-4E2C-95E1-601B20718C24}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{549B964F-FF32-493D-8ECA-37D2DA17F178}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95611AF2-4575-4FD9-A624-4C87522C6067}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB9747DB-1F49-4310-8D7F-9EA94834A746}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70C681E6-9A1D-4313-8207-23814A13B26D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71BB5656-5E76-4601-BB58-DBBEF8005AC4}"/>
 </file>
</xml_diff>